<commit_message>
not sure waht the changes were
</commit_message>
<xml_diff>
--- a/Output2.xlsx
+++ b/Output2.xlsx
@@ -7028,7 +7028,7 @@
         <v>2071</v>
       </c>
       <c r="E3">
-        <v>2071</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -7092,7 +7092,7 @@
         <v>2100</v>
       </c>
       <c r="E5">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -7336,7 +7336,7 @@
         <v>2102</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -7432,7 +7432,7 @@
         <v>2104</v>
       </c>
       <c r="E16">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -7496,7 +7496,7 @@
         <v>2091</v>
       </c>
       <c r="E18">
-        <v>2091</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -7528,7 +7528,7 @@
         <v>2092</v>
       </c>
       <c r="E19">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -7560,7 +7560,7 @@
         <v>2093</v>
       </c>
       <c r="E20">
-        <v>2093</v>
+        <v>1</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -7656,7 +7656,7 @@
         <v>2106</v>
       </c>
       <c r="E23">
-        <v>2106</v>
+        <v>1</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -7688,7 +7688,7 @@
         <v>2095</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2095</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -8060,7 +8060,7 @@
         <v>2108</v>
       </c>
       <c r="E36">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -8188,7 +8188,7 @@
         <v>2067</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>2067</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>2084</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2084</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -8316,7 +8316,7 @@
         <v>2098</v>
       </c>
       <c r="E44">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -8444,7 +8444,7 @@
         <v>2091</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>2091</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -8476,7 +8476,7 @@
         <v>2092</v>
       </c>
       <c r="E49">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -8528,7 +8528,7 @@
         <v>2100</v>
       </c>
       <c r="E51">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
@@ -8976,7 +8976,7 @@
         <v>2077</v>
       </c>
       <c r="E65">
-        <v>2077</v>
+        <v>1</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -9072,7 +9072,7 @@
         <v>2089</v>
       </c>
       <c r="E68">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -9424,7 +9424,7 @@
         <v>2104</v>
       </c>
       <c r="E79">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
@@ -9456,7 +9456,7 @@
         <v>2105</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -9520,7 +9520,7 @@
         <v>2106</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -9816,7 +9816,7 @@
         <v>2108</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
@@ -9848,7 +9848,7 @@
         <v>2109</v>
       </c>
       <c r="E93">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -9880,7 +9880,7 @@
         <v>2100</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
@@ -9964,7 +9964,7 @@
         <v>2101</v>
       </c>
       <c r="E97">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -10252,7 +10252,7 @@
         <v>2098</v>
       </c>
       <c r="E106">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F106" t="b">
         <v>0</v>
@@ -10956,7 +10956,7 @@
         <v>2107</v>
       </c>
       <c r="E128">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F128" t="b">
         <v>0</v>
@@ -11148,7 +11148,7 @@
         <v>2082</v>
       </c>
       <c r="E134">
-        <v>1</v>
+        <v>2082</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
@@ -11467,8 +11467,8 @@
       <c r="D144">
         <v>2043</v>
       </c>
-      <c r="E144">
-        <v>2043</v>
+      <c r="E144" t="b">
+        <v>0</v>
       </c>
       <c r="F144" t="b">
         <v>0</v>
@@ -12940,7 +12940,7 @@
         <v>2108</v>
       </c>
       <c r="E190">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F190" t="b">
         <v>0</v>
@@ -14124,7 +14124,7 @@
         <v>2059</v>
       </c>
       <c r="E227">
-        <v>1</v>
+        <v>2059</v>
       </c>
       <c r="F227" t="b">
         <v>0</v>
@@ -15500,7 +15500,7 @@
         <v>2109</v>
       </c>
       <c r="E270">
-        <v>1</v>
+        <v>2109</v>
       </c>
       <c r="F270" t="b">
         <v>0</v>
@@ -15595,8 +15595,8 @@
       <c r="D273">
         <v>2100</v>
       </c>
-      <c r="E273">
-        <v>2100</v>
+      <c r="E273" t="b">
+        <v>0</v>
       </c>
       <c r="F273" t="b">
         <v>0</v>
@@ -16172,7 +16172,7 @@
         <v>2062</v>
       </c>
       <c r="E291">
-        <v>2062</v>
+        <v>1</v>
       </c>
       <c r="F291" t="b">
         <v>0</v>
@@ -17291,8 +17291,8 @@
       <c r="D326">
         <v>2059</v>
       </c>
-      <c r="E326" t="b">
-        <v>0</v>
+      <c r="E326">
+        <v>2059</v>
       </c>
       <c r="F326" t="b">
         <v>0</v>
@@ -18124,7 +18124,7 @@
         <v>2091</v>
       </c>
       <c r="E352">
-        <v>2091</v>
+        <v>1</v>
       </c>
       <c r="F352" t="b">
         <v>0</v>
@@ -18732,7 +18732,7 @@
         <v>2101</v>
       </c>
       <c r="E371">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F371" t="b">
         <v>0</v>
@@ -18764,7 +18764,7 @@
         <v>2102</v>
       </c>
       <c r="E372">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F372" t="b">
         <v>0</v>
@@ -19820,7 +19820,7 @@
         <v>2092</v>
       </c>
       <c r="E405">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F405" t="b">
         <v>0</v>
@@ -19980,7 +19980,7 @@
         <v>2104</v>
       </c>
       <c r="E410">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F410" t="b">
         <v>0</v>
@@ -20012,7 +20012,7 @@
         <v>2105</v>
       </c>
       <c r="E411">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F411" t="b">
         <v>0</v>
@@ -20160,7 +20160,7 @@
         <v>2108</v>
       </c>
       <c r="E416">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F416" t="b">
         <v>0</v>
@@ -20372,7 +20372,7 @@
         <v>2100</v>
       </c>
       <c r="E423">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F423" t="b">
         <v>0</v>
@@ -20692,7 +20692,7 @@
         <v>2101</v>
       </c>
       <c r="E433">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F433" t="b">
         <v>0</v>
@@ -20756,7 +20756,7 @@
         <v>2102</v>
       </c>
       <c r="E435">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F435" t="b">
         <v>0</v>
@@ -21204,7 +21204,7 @@
         <v>2075</v>
       </c>
       <c r="E449">
-        <v>1</v>
+        <v>2075</v>
       </c>
       <c r="F449" t="b">
         <v>0</v>
@@ -21960,7 +21960,7 @@
         <v>2103</v>
       </c>
       <c r="E473">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F473" t="b">
         <v>0</v>
@@ -22280,7 +22280,7 @@
         <v>2040</v>
       </c>
       <c r="E483">
-        <v>2040</v>
+        <v>1</v>
       </c>
       <c r="F483" t="b">
         <v>0</v>
@@ -22376,7 +22376,7 @@
         <v>2030</v>
       </c>
       <c r="E486">
-        <v>2030</v>
+        <v>1</v>
       </c>
       <c r="F486" t="b">
         <v>0</v>
@@ -22408,7 +22408,7 @@
         <v>2107</v>
       </c>
       <c r="E487">
-        <v>2107</v>
+        <v>1</v>
       </c>
       <c r="F487" t="b">
         <v>0</v>
@@ -22504,7 +22504,7 @@
         <v>2096</v>
       </c>
       <c r="E490">
-        <v>1</v>
+        <v>2096</v>
       </c>
       <c r="F490" t="b">
         <v>0</v>
@@ -22920,7 +22920,7 @@
         <v>2109</v>
       </c>
       <c r="E503">
-        <v>1</v>
+        <v>2109</v>
       </c>
       <c r="F503" t="b">
         <v>0</v>
@@ -23112,7 +23112,7 @@
         <v>2099</v>
       </c>
       <c r="E509">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F509" t="b">
         <v>0</v>
@@ -23144,7 +23144,7 @@
         <v>2101</v>
       </c>
       <c r="E510">
-        <v>1</v>
+        <v>2101</v>
       </c>
       <c r="F510" t="b">
         <v>0</v>
@@ -24016,7 +24016,7 @@
         <v>2103</v>
       </c>
       <c r="E538">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F538" t="b">
         <v>0</v>
@@ -24304,7 +24304,7 @@
         <v>2092</v>
       </c>
       <c r="E547">
-        <v>1</v>
+        <v>2092</v>
       </c>
       <c r="F547" t="b">
         <v>0</v>
@@ -24368,7 +24368,7 @@
         <v>2093</v>
       </c>
       <c r="E549">
-        <v>1</v>
+        <v>2093</v>
       </c>
       <c r="F549" t="b">
         <v>0</v>
@@ -24400,7 +24400,7 @@
         <v>2104</v>
       </c>
       <c r="E550">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F550" t="b">
         <v>0</v>
@@ -24592,7 +24592,7 @@
         <v>2106</v>
       </c>
       <c r="E556">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F556" t="b">
         <v>0</v>
@@ -24752,7 +24752,7 @@
         <v>2108</v>
       </c>
       <c r="E561">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F561" t="b">
         <v>0</v>
@@ -24816,7 +24816,7 @@
         <v>2109</v>
       </c>
       <c r="E563">
-        <v>1</v>
+        <v>2109</v>
       </c>
       <c r="F563" t="b">
         <v>0</v>
@@ -24880,7 +24880,7 @@
         <v>2101</v>
       </c>
       <c r="E565">
-        <v>1</v>
+        <v>2101</v>
       </c>
       <c r="F565" t="b">
         <v>0</v>
@@ -25008,7 +25008,7 @@
         <v>2095</v>
       </c>
       <c r="E569">
-        <v>2095</v>
+        <v>1</v>
       </c>
       <c r="F569" t="b">
         <v>0</v>
@@ -25232,7 +25232,7 @@
         <v>2098</v>
       </c>
       <c r="E576">
-        <v>1</v>
+        <v>2098</v>
       </c>
       <c r="F576" t="b">
         <v>0</v>
@@ -25360,7 +25360,7 @@
         <v>2104</v>
       </c>
       <c r="E580">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F580" t="b">
         <v>0</v>
@@ -25424,7 +25424,7 @@
         <v>2105</v>
       </c>
       <c r="E582">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F582" t="b">
         <v>0</v>
@@ -25552,7 +25552,7 @@
         <v>2106</v>
       </c>
       <c r="E586">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F586" t="b">
         <v>0</v>
@@ -25584,7 +25584,7 @@
         <v>2089</v>
       </c>
       <c r="E587">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F587" t="b">
         <v>0</v>
@@ -25616,7 +25616,7 @@
         <v>2107</v>
       </c>
       <c r="E588">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F588" t="b">
         <v>0</v>
@@ -25680,7 +25680,7 @@
         <v>2109</v>
       </c>
       <c r="E590">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F590" t="b">
         <v>0</v>
@@ -25904,7 +25904,7 @@
         <v>2103</v>
       </c>
       <c r="E597">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F597" t="b">
         <v>0</v>
@@ -25936,7 +25936,7 @@
         <v>2104</v>
       </c>
       <c r="E598">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F598" t="b">
         <v>0</v>
@@ -26064,7 +26064,7 @@
         <v>2079</v>
       </c>
       <c r="E602">
-        <v>1</v>
+        <v>2079</v>
       </c>
       <c r="F602" t="b">
         <v>0</v>
@@ -26224,7 +26224,7 @@
         <v>2091</v>
       </c>
       <c r="E607">
-        <v>1</v>
+        <v>2091</v>
       </c>
       <c r="F607" t="b">
         <v>0</v>
@@ -26320,7 +26320,7 @@
         <v>2093</v>
       </c>
       <c r="E610">
-        <v>1</v>
+        <v>2093</v>
       </c>
       <c r="F610" t="b">
         <v>0</v>
@@ -26352,7 +26352,7 @@
         <v>2094</v>
       </c>
       <c r="E611">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F611" t="b">
         <v>0</v>
@@ -26416,7 +26416,7 @@
         <v>2106</v>
       </c>
       <c r="E613">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F613" t="b">
         <v>0</v>
@@ -26509,7 +26509,7 @@
         <v>2107</v>
       </c>
       <c r="E616">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F616" t="b">
         <v>0</v>
@@ -26605,7 +26605,7 @@
         <v>2109</v>
       </c>
       <c r="E619">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F619" t="b">
         <v>0</v>
@@ -27189,7 +27189,7 @@
         <v>2100</v>
       </c>
       <c r="E638">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F638" t="b">
         <v>0</v>
@@ -28137,7 +28137,7 @@
         <v>2060</v>
       </c>
       <c r="E668">
-        <v>1</v>
+        <v>2060</v>
       </c>
       <c r="F668" t="b">
         <v>0</v>
@@ -29673,7 +29673,7 @@
         <v>2063</v>
       </c>
       <c r="E716">
-        <v>1</v>
+        <v>2063</v>
       </c>
       <c r="F716" t="b">
         <v>0</v>
@@ -30057,7 +30057,7 @@
         <v>2099</v>
       </c>
       <c r="E728">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F728" t="b">
         <v>0</v>
@@ -30217,7 +30217,7 @@
         <v>2086</v>
       </c>
       <c r="E733">
-        <v>2086</v>
+        <v>1</v>
       </c>
       <c r="F733" t="b">
         <v>0</v>
@@ -30441,7 +30441,7 @@
         <v>2102</v>
       </c>
       <c r="E740">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F740" t="b">
         <v>0</v>
@@ -30825,7 +30825,7 @@
         <v>2109</v>
       </c>
       <c r="E752">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F752" t="b">
         <v>0</v>
@@ -30857,7 +30857,7 @@
         <v>2095</v>
       </c>
       <c r="E753">
-        <v>2095</v>
+        <v>1</v>
       </c>
       <c r="F753" t="b">
         <v>0</v>
@@ -30973,7 +30973,7 @@
         <v>2096</v>
       </c>
       <c r="E757">
-        <v>1</v>
+        <v>2096</v>
       </c>
       <c r="F757" t="b">
         <v>0</v>
@@ -31037,7 +31037,7 @@
         <v>2088</v>
       </c>
       <c r="E759">
-        <v>1</v>
+        <v>2088</v>
       </c>
       <c r="F759" t="b">
         <v>0</v>
@@ -31069,7 +31069,7 @@
         <v>2098</v>
       </c>
       <c r="E760">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F760" t="b">
         <v>0</v>
@@ -31197,7 +31197,7 @@
         <v>2100</v>
       </c>
       <c r="E764">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F764" t="b">
         <v>0</v>
@@ -31261,7 +31261,7 @@
         <v>2091</v>
       </c>
       <c r="E766">
-        <v>1</v>
+        <v>2091</v>
       </c>
       <c r="F766" t="b">
         <v>0</v>
@@ -31325,7 +31325,7 @@
         <v>2089</v>
       </c>
       <c r="E768">
-        <v>1</v>
+        <v>2089</v>
       </c>
       <c r="F768" t="b">
         <v>0</v>
@@ -31357,7 +31357,7 @@
         <v>2064</v>
       </c>
       <c r="E769">
-        <v>2064</v>
+        <v>1</v>
       </c>
       <c r="F769" t="b">
         <v>0</v>
@@ -31517,7 +31517,7 @@
         <v>2095</v>
       </c>
       <c r="E774">
-        <v>1</v>
+        <v>2095</v>
       </c>
       <c r="F774" t="b">
         <v>0</v>
@@ -31549,7 +31549,7 @@
         <v>2096</v>
       </c>
       <c r="E775">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F775" t="b">
         <v>0</v>
@@ -31741,7 +31741,7 @@
         <v>2091</v>
       </c>
       <c r="E781">
-        <v>2091</v>
+        <v>1</v>
       </c>
       <c r="F781" t="b">
         <v>0</v>
@@ -31773,7 +31773,7 @@
         <v>2092</v>
       </c>
       <c r="E782">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F782" t="b">
         <v>0</v>
@@ -31805,7 +31805,7 @@
         <v>2079</v>
       </c>
       <c r="E783">
-        <v>1</v>
+        <v>2079</v>
       </c>
       <c r="F783" t="b">
         <v>0</v>
@@ -32442,7 +32442,7 @@
         <v>2108</v>
       </c>
       <c r="E803">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F803" t="b">
         <v>0</v>
@@ -32474,7 +32474,7 @@
         <v>2109</v>
       </c>
       <c r="E804">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F804" t="b">
         <v>0</v>
@@ -32602,7 +32602,7 @@
         <v>2087</v>
       </c>
       <c r="E808">
-        <v>1</v>
+        <v>2087</v>
       </c>
       <c r="F808" t="b">
         <v>0</v>
@@ -32730,7 +32730,7 @@
         <v>2102</v>
       </c>
       <c r="E812">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F812" t="b">
         <v>0</v>
@@ -32878,7 +32878,7 @@
         <v>2089</v>
       </c>
       <c r="E817">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F817" t="b">
         <v>0</v>
@@ -33070,7 +33070,7 @@
         <v>2103</v>
       </c>
       <c r="E823">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F823" t="b">
         <v>0</v>
@@ -33102,7 +33102,7 @@
         <v>2096</v>
       </c>
       <c r="E824">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F824" t="b">
         <v>0</v>
@@ -33154,7 +33154,7 @@
         <v>2097</v>
       </c>
       <c r="E826">
-        <v>1</v>
+        <v>2097</v>
       </c>
       <c r="F826" t="b">
         <v>0</v>
@@ -33186,7 +33186,7 @@
         <v>2098</v>
       </c>
       <c r="E827">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F827" t="b">
         <v>0</v>
@@ -33474,7 +33474,7 @@
         <v>2065</v>
       </c>
       <c r="E836">
-        <v>2065</v>
+        <v>1</v>
       </c>
       <c r="F836" t="b">
         <v>0</v>
@@ -33602,7 +33602,7 @@
         <v>2105</v>
       </c>
       <c r="E840">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F840" t="b">
         <v>0</v>
@@ -33814,7 +33814,7 @@
         <v>2094</v>
       </c>
       <c r="E847">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F847" t="b">
         <v>0</v>
@@ -34038,7 +34038,7 @@
         <v>2095</v>
       </c>
       <c r="E854">
-        <v>2095</v>
+        <v>1</v>
       </c>
       <c r="F854" t="b">
         <v>0</v>
@@ -34166,7 +34166,7 @@
         <v>2096</v>
       </c>
       <c r="E858">
-        <v>1</v>
+        <v>2096</v>
       </c>
       <c r="F858" t="b">
         <v>0</v>
@@ -34294,7 +34294,7 @@
         <v>2107</v>
       </c>
       <c r="E862">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F862" t="b">
         <v>0</v>
@@ -34326,7 +34326,7 @@
         <v>2108</v>
       </c>
       <c r="E863">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F863" t="b">
         <v>0</v>
@@ -34518,7 +34518,7 @@
         <v>2100</v>
       </c>
       <c r="E869">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F869" t="b">
         <v>0</v>
@@ -34550,7 +34550,7 @@
         <v>2101</v>
       </c>
       <c r="E870">
-        <v>1</v>
+        <v>2101</v>
       </c>
       <c r="F870" t="b">
         <v>0</v>
@@ -34634,7 +34634,7 @@
         <v>2102</v>
       </c>
       <c r="E873">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F873" t="b">
         <v>0</v>
@@ -34814,7 +34814,7 @@
         <v>2094</v>
       </c>
       <c r="E879">
-        <v>2094</v>
+        <v>1</v>
       </c>
       <c r="F879" t="b">
         <v>0</v>
@@ -34910,7 +34910,7 @@
         <v>2096</v>
       </c>
       <c r="E882">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F882" t="b">
         <v>0</v>
@@ -34942,7 +34942,7 @@
         <v>2103</v>
       </c>
       <c r="E883">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F883" t="b">
         <v>0</v>
@@ -34974,7 +34974,7 @@
         <v>2084</v>
       </c>
       <c r="E884">
-        <v>1</v>
+        <v>2084</v>
       </c>
       <c r="F884" t="b">
         <v>0</v>
@@ -35102,7 +35102,7 @@
         <v>2098</v>
       </c>
       <c r="E888">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F888" t="b">
         <v>0</v>
@@ -35166,7 +35166,7 @@
         <v>2104</v>
       </c>
       <c r="E890">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F890" t="b">
         <v>0</v>
@@ -35198,7 +35198,7 @@
         <v>2088</v>
       </c>
       <c r="E891">
-        <v>1</v>
+        <v>2088</v>
       </c>
       <c r="F891" t="b">
         <v>0</v>
@@ -35294,7 +35294,7 @@
         <v>2091</v>
       </c>
       <c r="E894">
-        <v>1</v>
+        <v>2091</v>
       </c>
       <c r="F894" t="b">
         <v>0</v>
@@ -35378,7 +35378,7 @@
         <v>2105</v>
       </c>
       <c r="E897">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F897" t="b">
         <v>0</v>
@@ -35538,7 +35538,7 @@
         <v>2094</v>
       </c>
       <c r="E902">
-        <v>2094</v>
+        <v>1</v>
       </c>
       <c r="F902" t="b">
         <v>0</v>
@@ -35602,7 +35602,7 @@
         <v>2107</v>
       </c>
       <c r="E904">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F904" t="b">
         <v>0</v>
@@ -35954,7 +35954,7 @@
         <v>2084</v>
       </c>
       <c r="E915">
-        <v>1</v>
+        <v>2084</v>
       </c>
       <c r="F915" t="b">
         <v>0</v>
@@ -36018,7 +36018,7 @@
         <v>2108</v>
       </c>
       <c r="E917">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F917" t="b">
         <v>0</v>
@@ -36082,7 +36082,7 @@
         <v>2098</v>
       </c>
       <c r="E919">
-        <v>1</v>
+        <v>2098</v>
       </c>
       <c r="F919" t="b">
         <v>0</v>
@@ -36210,7 +36210,7 @@
         <v>2086</v>
       </c>
       <c r="E923">
-        <v>2086</v>
+        <v>1</v>
       </c>
       <c r="F923" t="b">
         <v>0</v>
@@ -36306,7 +36306,7 @@
         <v>2090</v>
       </c>
       <c r="E926">
-        <v>1</v>
+        <v>2090</v>
       </c>
       <c r="F926" t="b">
         <v>0</v>
@@ -36338,7 +36338,7 @@
         <v>2102</v>
       </c>
       <c r="E927">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F927" t="b">
         <v>0</v>
@@ -36678,7 +36678,7 @@
         <v>2076</v>
       </c>
       <c r="E938">
-        <v>2076</v>
+        <v>1</v>
       </c>
       <c r="F938" t="b">
         <v>0</v>
@@ -36710,7 +36710,7 @@
         <v>2104</v>
       </c>
       <c r="E939">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F939" t="b">
         <v>0</v>
@@ -36742,7 +36742,7 @@
         <v>2105</v>
       </c>
       <c r="E940">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F940" t="b">
         <v>0</v>
@@ -36774,7 +36774,7 @@
         <v>2106</v>
       </c>
       <c r="E941">
-        <v>2106</v>
+        <v>1</v>
       </c>
       <c r="F941" t="b">
         <v>0</v>
@@ -36838,7 +36838,7 @@
         <v>2107</v>
       </c>
       <c r="E943">
-        <v>2107</v>
+        <v>1</v>
       </c>
       <c r="F943" t="b">
         <v>0</v>
@@ -36870,7 +36870,7 @@
         <v>2108</v>
       </c>
       <c r="E944">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F944" t="b">
         <v>0</v>
@@ -36998,7 +36998,7 @@
         <v>2090</v>
       </c>
       <c r="E948">
-        <v>1</v>
+        <v>2090</v>
       </c>
       <c r="F948" t="b">
         <v>0</v>
@@ -37062,7 +37062,7 @@
         <v>2109</v>
       </c>
       <c r="E950">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F950" t="b">
         <v>0</v>
@@ -37158,7 +37158,7 @@
         <v>2100</v>
       </c>
       <c r="E953">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F953" t="b">
         <v>0</v>
@@ -37190,7 +37190,7 @@
         <v>2101</v>
       </c>
       <c r="E954">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F954" t="b">
         <v>0</v>
@@ -37318,7 +37318,7 @@
         <v>2102</v>
       </c>
       <c r="E958">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F958" t="b">
         <v>0</v>
@@ -37350,7 +37350,7 @@
         <v>2095</v>
       </c>
       <c r="E959">
-        <v>2095</v>
+        <v>1</v>
       </c>
       <c r="F959" t="b">
         <v>0</v>
@@ -37414,7 +37414,7 @@
         <v>2096</v>
       </c>
       <c r="E961">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F961" t="b">
         <v>0</v>
@@ -37478,7 +37478,7 @@
         <v>2103</v>
       </c>
       <c r="E963">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F963" t="b">
         <v>0</v>
@@ -37510,7 +37510,7 @@
         <v>2089</v>
       </c>
       <c r="E964">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F964" t="b">
         <v>0</v>
@@ -37606,7 +37606,7 @@
         <v>2097</v>
       </c>
       <c r="E967">
-        <v>2097</v>
+        <v>1</v>
       </c>
       <c r="F967" t="b">
         <v>0</v>
@@ -37797,8 +37797,8 @@
       <c r="D973">
         <v>2107</v>
       </c>
-      <c r="E973" t="b">
-        <v>0</v>
+      <c r="E973">
+        <v>1</v>
       </c>
       <c r="F973" t="b">
         <v>0</v>
@@ -37894,7 +37894,7 @@
         <v>2108</v>
       </c>
       <c r="E976">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F976" t="b">
         <v>0</v>
@@ -38150,7 +38150,7 @@
         <v>2099</v>
       </c>
       <c r="E984">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F984" t="b">
         <v>0</v>
@@ -38342,7 +38342,7 @@
         <v>2104</v>
       </c>
       <c r="E990">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F990" t="b">
         <v>0</v>
@@ -38406,7 +38406,7 @@
         <v>2106</v>
       </c>
       <c r="E992">
-        <v>2106</v>
+        <v>1</v>
       </c>
       <c r="F992" t="b">
         <v>0</v>
@@ -38438,7 +38438,7 @@
         <v>2092</v>
       </c>
       <c r="E993">
-        <v>1</v>
+        <v>2092</v>
       </c>
       <c r="F993" t="b">
         <v>0</v>
@@ -38554,7 +38554,7 @@
         <v>2107</v>
       </c>
       <c r="E997">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F997" t="b">
         <v>0</v>
@@ -38586,7 +38586,7 @@
         <v>2094</v>
       </c>
       <c r="E998">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F998" t="b">
         <v>0</v>
@@ -38714,7 +38714,7 @@
         <v>2108</v>
       </c>
       <c r="E1002">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F1002" t="b">
         <v>0</v>
@@ -38906,7 +38906,7 @@
         <v>2101</v>
       </c>
       <c r="E1008">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F1008" t="b">
         <v>0</v>
@@ -38938,7 +38938,7 @@
         <v>2096</v>
       </c>
       <c r="E1009">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F1009" t="b">
         <v>0</v>
@@ -38970,7 +38970,7 @@
         <v>2097</v>
       </c>
       <c r="E1010">
-        <v>1</v>
+        <v>2097</v>
       </c>
       <c r="F1010" t="b">
         <v>0</v>
@@ -39086,7 +39086,7 @@
         <v>2098</v>
       </c>
       <c r="E1014">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F1014" t="b">
         <v>0</v>
@@ -39246,7 +39246,7 @@
         <v>2088</v>
       </c>
       <c r="E1019">
-        <v>1</v>
+        <v>2088</v>
       </c>
       <c r="F1019" t="b">
         <v>0</v>
@@ -39438,7 +39438,7 @@
         <v>2068</v>
       </c>
       <c r="E1025">
-        <v>1</v>
+        <v>2068</v>
       </c>
       <c r="F1025" t="b">
         <v>0</v>
@@ -39534,7 +39534,7 @@
         <v>2090</v>
       </c>
       <c r="E1028">
-        <v>2090</v>
+        <v>1</v>
       </c>
       <c r="F1028" t="b">
         <v>0</v>
@@ -39662,7 +39662,7 @@
         <v>2103</v>
       </c>
       <c r="E1032">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F1032" t="b">
         <v>0</v>
@@ -39822,7 +39822,7 @@
         <v>2104</v>
       </c>
       <c r="E1037">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F1037" t="b">
         <v>0</v>
@@ -40002,7 +40002,7 @@
         <v>2092</v>
       </c>
       <c r="E1043">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1043" t="b">
         <v>0</v>
@@ -40130,7 +40130,7 @@
         <v>2107</v>
       </c>
       <c r="E1047">
-        <v>2107</v>
+        <v>1</v>
       </c>
       <c r="F1047" t="b">
         <v>0</v>
@@ -40339,7 +40339,7 @@
         <v>2096</v>
       </c>
       <c r="E1054">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F1054" t="b">
         <v>0</v>
@@ -40531,7 +40531,7 @@
         <v>2099</v>
       </c>
       <c r="E1060">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F1060" t="b">
         <v>0</v>
@@ -40563,7 +40563,7 @@
         <v>2089</v>
       </c>
       <c r="E1061">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F1061" t="b">
         <v>0</v>
@@ -40595,7 +40595,7 @@
         <v>2100</v>
       </c>
       <c r="E1062">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F1062" t="b">
         <v>0</v>
@@ -40627,7 +40627,7 @@
         <v>2076</v>
       </c>
       <c r="E1063">
-        <v>1</v>
+        <v>2076</v>
       </c>
       <c r="F1063" t="b">
         <v>0</v>
@@ -40691,7 +40691,7 @@
         <v>2090</v>
       </c>
       <c r="E1065">
-        <v>1</v>
+        <v>2090</v>
       </c>
       <c r="F1065" t="b">
         <v>0</v>
@@ -40787,7 +40787,7 @@
         <v>2092</v>
       </c>
       <c r="E1068">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1068" t="b">
         <v>0</v>
@@ -40819,7 +40819,7 @@
         <v>2093</v>
       </c>
       <c r="E1069">
-        <v>2093</v>
+        <v>1</v>
       </c>
       <c r="F1069" t="b">
         <v>0</v>
@@ -41075,7 +41075,7 @@
         <v>2103</v>
       </c>
       <c r="E1077">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F1077" t="b">
         <v>0</v>
@@ -41491,7 +41491,7 @@
         <v>2090</v>
       </c>
       <c r="E1090">
-        <v>2090</v>
+        <v>1</v>
       </c>
       <c r="F1090" t="b">
         <v>0</v>
@@ -41683,7 +41683,7 @@
         <v>2106</v>
       </c>
       <c r="E1096">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F1096" t="b">
         <v>0</v>
@@ -41747,7 +41747,7 @@
         <v>2108</v>
       </c>
       <c r="E1098">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F1098" t="b">
         <v>0</v>
@@ -41811,7 +41811,7 @@
         <v>2109</v>
       </c>
       <c r="E1100">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F1100" t="b">
         <v>0</v>
@@ -41843,7 +41843,7 @@
         <v>2092</v>
       </c>
       <c r="E1101">
-        <v>1</v>
+        <v>2092</v>
       </c>
       <c r="F1101" t="b">
         <v>0</v>
@@ -41906,8 +41906,8 @@
       <c r="D1103">
         <v>2094</v>
       </c>
-      <c r="E1103">
-        <v>2094</v>
+      <c r="E1103" t="b">
+        <v>0</v>
       </c>
       <c r="F1103" t="b">
         <v>0</v>
@@ -42035,7 +42035,7 @@
         <v>2101</v>
       </c>
       <c r="E1107">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F1107" t="b">
         <v>0</v>
@@ -42355,7 +42355,7 @@
         <v>2105</v>
       </c>
       <c r="E1117">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F1117" t="b">
         <v>0</v>
@@ -42451,7 +42451,7 @@
         <v>2089</v>
       </c>
       <c r="E1120">
-        <v>1</v>
+        <v>2089</v>
       </c>
       <c r="F1120" t="b">
         <v>0</v>
@@ -42515,7 +42515,7 @@
         <v>2090</v>
       </c>
       <c r="E1122">
-        <v>2090</v>
+        <v>1</v>
       </c>
       <c r="F1122" t="b">
         <v>0</v>
@@ -42579,7 +42579,7 @@
         <v>2080</v>
       </c>
       <c r="E1124">
-        <v>1</v>
+        <v>2080</v>
       </c>
       <c r="F1124" t="b">
         <v>0</v>
@@ -42611,7 +42611,7 @@
         <v>2108</v>
       </c>
       <c r="E1125">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F1125" t="b">
         <v>0</v>
@@ -42707,7 +42707,7 @@
         <v>2100</v>
       </c>
       <c r="E1128">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F1128" t="b">
         <v>0</v>
@@ -42803,7 +42803,7 @@
         <v>2102</v>
       </c>
       <c r="E1131">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F1131" t="b">
         <v>0</v>
@@ -43283,7 +43283,7 @@
         <v>2099</v>
       </c>
       <c r="E1146">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F1146" t="b">
         <v>0</v>
@@ -43635,7 +43635,7 @@
         <v>2092</v>
       </c>
       <c r="E1157">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1157" t="b">
         <v>0</v>
@@ -43699,7 +43699,7 @@
         <v>2108</v>
       </c>
       <c r="E1159">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F1159" t="b">
         <v>0</v>
@@ -43859,7 +43859,7 @@
         <v>2094</v>
       </c>
       <c r="E1164">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F1164" t="b">
         <v>0</v>
@@ -44039,7 +44039,7 @@
         <v>2101</v>
       </c>
       <c r="E1170">
-        <v>1</v>
+        <v>2101</v>
       </c>
       <c r="F1170" t="b">
         <v>0</v>
@@ -44071,7 +44071,7 @@
         <v>2089</v>
       </c>
       <c r="E1171">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F1171" t="b">
         <v>0</v>
@@ -44135,7 +44135,7 @@
         <v>2102</v>
       </c>
       <c r="E1173">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F1173" t="b">
         <v>0</v>
@@ -44231,7 +44231,7 @@
         <v>2097</v>
       </c>
       <c r="E1176">
-        <v>1</v>
+        <v>2097</v>
       </c>
       <c r="F1176" t="b">
         <v>0</v>
@@ -44263,7 +44263,7 @@
         <v>2098</v>
       </c>
       <c r="E1177">
-        <v>1</v>
+        <v>2098</v>
       </c>
       <c r="F1177" t="b">
         <v>0</v>
@@ -44539,7 +44539,7 @@
         <v>2107</v>
       </c>
       <c r="E1186">
-        <v>2107</v>
+        <v>1</v>
       </c>
       <c r="F1186" t="b">
         <v>0</v>
@@ -44623,7 +44623,7 @@
         <v>2099</v>
       </c>
       <c r="E1189">
-        <v>1</v>
+        <v>2099</v>
       </c>
       <c r="F1189" t="b">
         <v>0</v>
@@ -44719,7 +44719,7 @@
         <v>2085</v>
       </c>
       <c r="E1192">
-        <v>2085</v>
+        <v>1</v>
       </c>
       <c r="F1192" t="b">
         <v>0</v>
@@ -45091,7 +45091,7 @@
         <v>2075</v>
       </c>
       <c r="E1204">
-        <v>1</v>
+        <v>2075</v>
       </c>
       <c r="F1204" t="b">
         <v>0</v>
@@ -45155,7 +45155,7 @@
         <v>2089</v>
       </c>
       <c r="E1206">
-        <v>1</v>
+        <v>2089</v>
       </c>
       <c r="F1206" t="b">
         <v>0</v>
@@ -45303,7 +45303,7 @@
         <v>2103</v>
       </c>
       <c r="E1211">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F1211" t="b">
         <v>0</v>
@@ -45399,7 +45399,7 @@
         <v>2104</v>
       </c>
       <c r="E1214">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F1214" t="b">
         <v>0</v>
@@ -45463,7 +45463,7 @@
         <v>2105</v>
       </c>
       <c r="E1216">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F1216" t="b">
         <v>0</v>
@@ -45687,7 +45687,7 @@
         <v>2077</v>
       </c>
       <c r="E1223">
-        <v>1</v>
+        <v>2077</v>
       </c>
       <c r="F1223" t="b">
         <v>0</v>
@@ -45751,7 +45751,7 @@
         <v>2082</v>
       </c>
       <c r="E1225">
-        <v>2082</v>
+        <v>1</v>
       </c>
       <c r="F1225" t="b">
         <v>0</v>
@@ -45975,7 +45975,7 @@
         <v>2097</v>
       </c>
       <c r="E1232">
-        <v>2097</v>
+        <v>1</v>
       </c>
       <c r="F1232" t="b">
         <v>0</v>
@@ -46787,7 +46787,7 @@
         <v>2090</v>
       </c>
       <c r="E1260">
-        <v>1</v>
+        <v>2090</v>
       </c>
       <c r="F1260" t="b">
         <v>0</v>
@@ -46819,7 +46819,7 @@
         <v>2108</v>
       </c>
       <c r="E1261">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F1261" t="b">
         <v>0</v>
@@ -46851,7 +46851,7 @@
         <v>2086</v>
       </c>
       <c r="E1262">
-        <v>1</v>
+        <v>2086</v>
       </c>
       <c r="F1262" t="b">
         <v>0</v>
@@ -46915,7 +46915,7 @@
         <v>2109</v>
       </c>
       <c r="E1264">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F1264" t="b">
         <v>0</v>
@@ -47011,7 +47011,7 @@
         <v>2100</v>
       </c>
       <c r="E1267">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F1267" t="b">
         <v>0</v>
@@ -47043,7 +47043,7 @@
         <v>2093</v>
       </c>
       <c r="E1268">
-        <v>2093</v>
+        <v>1</v>
       </c>
       <c r="F1268" t="b">
         <v>0</v>
@@ -47107,7 +47107,7 @@
         <v>2088</v>
       </c>
       <c r="E1270">
-        <v>1</v>
+        <v>2088</v>
       </c>
       <c r="F1270" t="b">
         <v>0</v>
@@ -47171,7 +47171,7 @@
         <v>2102</v>
       </c>
       <c r="E1272">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F1272" t="b">
         <v>0</v>
@@ -47203,7 +47203,7 @@
         <v>2094</v>
       </c>
       <c r="E1273">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F1273" t="b">
         <v>0</v>
@@ -47235,7 +47235,7 @@
         <v>2070</v>
       </c>
       <c r="E1274">
-        <v>1</v>
+        <v>2070</v>
       </c>
       <c r="F1274" t="b">
         <v>0</v>
@@ -47395,7 +47395,7 @@
         <v>2104</v>
       </c>
       <c r="E1279">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F1279" t="b">
         <v>0</v>
@@ -47427,7 +47427,7 @@
         <v>2105</v>
       </c>
       <c r="E1280">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F1280" t="b">
         <v>0</v>
@@ -47523,7 +47523,7 @@
         <v>2098</v>
       </c>
       <c r="E1283">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F1283" t="b">
         <v>0</v>
@@ -47651,7 +47651,7 @@
         <v>2090</v>
       </c>
       <c r="E1287">
-        <v>1</v>
+        <v>2090</v>
       </c>
       <c r="F1287" t="b">
         <v>0</v>
@@ -47971,7 +47971,7 @@
         <v>2107</v>
       </c>
       <c r="E1297">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F1297" t="b">
         <v>0</v>
@@ -48035,7 +48035,7 @@
         <v>2108</v>
       </c>
       <c r="E1299">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F1299" t="b">
         <v>0</v>
@@ -48066,8 +48066,8 @@
       <c r="D1300">
         <v>2109</v>
       </c>
-      <c r="E1300">
-        <v>2109</v>
+      <c r="E1300" t="b">
+        <v>0</v>
       </c>
       <c r="F1300" t="b">
         <v>0</v>
@@ -48131,7 +48131,7 @@
         <v>2100</v>
       </c>
       <c r="E1302">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F1302" t="b">
         <v>0</v>
@@ -48163,7 +48163,7 @@
         <v>2094</v>
       </c>
       <c r="E1303">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F1303" t="b">
         <v>0</v>
@@ -48279,7 +48279,7 @@
         <v>2087</v>
       </c>
       <c r="E1307">
-        <v>1</v>
+        <v>2087</v>
       </c>
       <c r="F1307" t="b">
         <v>0</v>
@@ -48503,7 +48503,7 @@
         <v>2099</v>
       </c>
       <c r="E1314">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F1314" t="b">
         <v>0</v>
@@ -49140,7 +49140,7 @@
         <v>2092</v>
       </c>
       <c r="E1334">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1334" t="b">
         <v>0</v>
@@ -49204,7 +49204,7 @@
         <v>2093</v>
       </c>
       <c r="E1336">
-        <v>2093</v>
+        <v>1</v>
       </c>
       <c r="F1336" t="b">
         <v>0</v>
@@ -49428,7 +49428,7 @@
         <v>2096</v>
       </c>
       <c r="E1343">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F1343" t="b">
         <v>0</v>
@@ -49556,7 +49556,7 @@
         <v>2070</v>
       </c>
       <c r="E1347">
-        <v>2070</v>
+        <v>1</v>
       </c>
       <c r="F1347" t="b">
         <v>0</v>
@@ -49588,7 +49588,7 @@
         <v>2098</v>
       </c>
       <c r="E1348">
-        <v>1</v>
+        <v>2098</v>
       </c>
       <c r="F1348" t="b">
         <v>0</v>
@@ -49620,7 +49620,7 @@
         <v>2071</v>
       </c>
       <c r="E1349">
-        <v>1</v>
+        <v>2071</v>
       </c>
       <c r="F1349" t="b">
         <v>0</v>
@@ -49844,7 +49844,7 @@
         <v>2091</v>
       </c>
       <c r="E1356">
-        <v>1</v>
+        <v>2091</v>
       </c>
       <c r="F1356" t="b">
         <v>0</v>
@@ -49908,7 +49908,7 @@
         <v>2075</v>
       </c>
       <c r="E1358">
-        <v>2075</v>
+        <v>1</v>
       </c>
       <c r="F1358" t="b">
         <v>0</v>
@@ -49972,7 +49972,7 @@
         <v>2093</v>
       </c>
       <c r="E1360">
-        <v>2093</v>
+        <v>1</v>
       </c>
       <c r="F1360" t="b">
         <v>0</v>
@@ -50004,7 +50004,7 @@
         <v>2085</v>
       </c>
       <c r="E1361">
-        <v>2085</v>
+        <v>1</v>
       </c>
       <c r="F1361" t="b">
         <v>0</v>
@@ -50036,7 +50036,7 @@
         <v>2104</v>
       </c>
       <c r="E1362">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F1362" t="b">
         <v>0</v>
@@ -50068,7 +50068,7 @@
         <v>2094</v>
       </c>
       <c r="E1363">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F1363" t="b">
         <v>0</v>
@@ -50132,7 +50132,7 @@
         <v>2095</v>
       </c>
       <c r="E1365">
-        <v>1</v>
+        <v>2095</v>
       </c>
       <c r="F1365" t="b">
         <v>0</v>
@@ -50196,7 +50196,7 @@
         <v>2106</v>
       </c>
       <c r="E1367">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F1367" t="b">
         <v>0</v>
@@ -50228,7 +50228,7 @@
         <v>2096</v>
       </c>
       <c r="E1368">
-        <v>2096</v>
+        <v>1</v>
       </c>
       <c r="F1368" t="b">
         <v>0</v>
@@ -50292,7 +50292,7 @@
         <v>2097</v>
       </c>
       <c r="E1370">
-        <v>2097</v>
+        <v>1</v>
       </c>
       <c r="F1370" t="b">
         <v>0</v>
@@ -50548,7 +50548,7 @@
         <v>2099</v>
       </c>
       <c r="E1378">
-        <v>1</v>
+        <v>2099</v>
       </c>
       <c r="F1378" t="b">
         <v>0</v>
@@ -50644,7 +50644,7 @@
         <v>2100</v>
       </c>
       <c r="E1381">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F1381" t="b">
         <v>0</v>
@@ -50740,7 +50740,7 @@
         <v>2102</v>
       </c>
       <c r="E1384">
-        <v>1</v>
+        <v>2102</v>
       </c>
       <c r="F1384" t="b">
         <v>0</v>
@@ -50804,7 +50804,7 @@
         <v>2092</v>
       </c>
       <c r="E1386">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1386" t="b">
         <v>0</v>
@@ -50868,7 +50868,7 @@
         <v>2104</v>
       </c>
       <c r="E1388">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F1388" t="b">
         <v>0</v>
@@ -50932,7 +50932,7 @@
         <v>2094</v>
       </c>
       <c r="E1390">
-        <v>1</v>
+        <v>2094</v>
       </c>
       <c r="F1390" t="b">
         <v>0</v>
@@ -51124,7 +51124,7 @@
         <v>2106</v>
       </c>
       <c r="E1396">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F1396" t="b">
         <v>0</v>
@@ -51156,7 +51156,7 @@
         <v>2107</v>
       </c>
       <c r="E1397">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F1397" t="b">
         <v>0</v>
@@ -51981,7 +51981,7 @@
         <v>2108</v>
       </c>
       <c r="E1424">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F1424" t="b">
         <v>0</v>
@@ -52265,7 +52265,7 @@
         <v>2099</v>
       </c>
       <c r="E1434">
-        <v>1</v>
+        <v>2099</v>
       </c>
       <c r="F1434" t="b">
         <v>0</v>
@@ -52381,7 +52381,7 @@
         <v>2065</v>
       </c>
       <c r="E1438">
-        <v>2065</v>
+        <v>1</v>
       </c>
       <c r="F1438" t="b">
         <v>0</v>
@@ -52829,7 +52829,7 @@
         <v>2092</v>
       </c>
       <c r="E1452">
-        <v>2092</v>
+        <v>1</v>
       </c>
       <c r="F1452" t="b">
         <v>0</v>
@@ -52893,7 +52893,7 @@
         <v>2094</v>
       </c>
       <c r="E1454">
-        <v>2094</v>
+        <v>1</v>
       </c>
       <c r="F1454" t="b">
         <v>0</v>
@@ -53085,7 +53085,7 @@
         <v>2088</v>
       </c>
       <c r="E1460">
-        <v>1</v>
+        <v>2088</v>
       </c>
       <c r="F1460" t="b">
         <v>0</v>
@@ -53149,7 +53149,7 @@
         <v>2096</v>
       </c>
       <c r="E1462">
-        <v>1</v>
+        <v>2096</v>
       </c>
       <c r="F1462" t="b">
         <v>0</v>
@@ -53181,7 +53181,7 @@
         <v>2097</v>
       </c>
       <c r="E1463">
-        <v>2097</v>
+        <v>1</v>
       </c>
       <c r="F1463" t="b">
         <v>0</v>
@@ -53213,7 +53213,7 @@
         <v>2089</v>
       </c>
       <c r="E1464">
-        <v>2089</v>
+        <v>1</v>
       </c>
       <c r="F1464" t="b">
         <v>0</v>
@@ -53245,7 +53245,7 @@
         <v>2098</v>
       </c>
       <c r="E1465">
-        <v>1</v>
+        <v>2098</v>
       </c>
       <c r="F1465" t="b">
         <v>0</v>
@@ -53469,7 +53469,7 @@
         <v>2099</v>
       </c>
       <c r="E1472">
-        <v>2099</v>
+        <v>1</v>
       </c>
       <c r="F1472" t="b">
         <v>0</v>
@@ -53597,7 +53597,7 @@
         <v>2086</v>
       </c>
       <c r="E1476">
-        <v>1</v>
+        <v>2086</v>
       </c>
       <c r="F1476" t="b">
         <v>0</v>
@@ -53661,7 +53661,7 @@
         <v>2088</v>
       </c>
       <c r="E1478">
-        <v>2088</v>
+        <v>1</v>
       </c>
       <c r="F1478" t="b">
         <v>0</v>
@@ -53693,7 +53693,7 @@
         <v>2090</v>
       </c>
       <c r="E1479">
-        <v>2090</v>
+        <v>1</v>
       </c>
       <c r="F1479" t="b">
         <v>0</v>
@@ -53818,7 +53818,7 @@
         <v>2075</v>
       </c>
       <c r="E1483">
-        <v>1</v>
+        <v>2075</v>
       </c>
       <c r="F1483" t="b">
         <v>0</v>
@@ -53850,7 +53850,7 @@
         <v>2091</v>
       </c>
       <c r="E1484">
-        <v>2091</v>
+        <v>1</v>
       </c>
       <c r="F1484" t="b">
         <v>0</v>
@@ -53913,8 +53913,8 @@
       <c r="D1486">
         <v>2093</v>
       </c>
-      <c r="E1486">
-        <v>1</v>
+      <c r="E1486" t="b">
+        <v>0</v>
       </c>
       <c r="F1486" t="b">
         <v>0</v>
@@ -54074,7 +54074,7 @@
         <v>2100</v>
       </c>
       <c r="E1491">
-        <v>1</v>
+        <v>2100</v>
       </c>
       <c r="F1491" t="b">
         <v>0</v>
@@ -54106,7 +54106,7 @@
         <v>2095</v>
       </c>
       <c r="E1492">
-        <v>1</v>
+        <v>2095</v>
       </c>
       <c r="F1492" t="b">
         <v>0</v>
@@ -54170,7 +54170,7 @@
         <v>2102</v>
       </c>
       <c r="E1494">
-        <v>2102</v>
+        <v>1</v>
       </c>
       <c r="F1494" t="b">
         <v>0</v>
@@ -54266,7 +54266,7 @@
         <v>2104</v>
       </c>
       <c r="E1497">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F1497" t="b">
         <v>0</v>
@@ -54298,7 +54298,7 @@
         <v>2081</v>
       </c>
       <c r="E1498">
-        <v>2081</v>
+        <v>1</v>
       </c>
       <c r="F1498" t="b">
         <v>0</v>
@@ -54554,7 +54554,7 @@
         <v>2083</v>
       </c>
       <c r="E1506">
-        <v>2083</v>
+        <v>1</v>
       </c>
       <c r="F1506" t="b">
         <v>0</v>
@@ -54618,7 +54618,7 @@
         <v>2106</v>
       </c>
       <c r="E1508">
-        <v>2106</v>
+        <v>1</v>
       </c>
       <c r="F1508" t="b">
         <v>0</v>
@@ -54938,7 +54938,7 @@
         <v>2097</v>
       </c>
       <c r="E1518">
-        <v>1</v>
+        <v>2097</v>
       </c>
       <c r="F1518" t="b">
         <v>0</v>
@@ -55226,7 +55226,7 @@
         <v>2108</v>
       </c>
       <c r="E1527">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F1527" t="b">
         <v>0</v>
@@ -55854,7 +55854,7 @@
         <v>2101</v>
       </c>
       <c r="E1547">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F1547" t="b">
         <v>0</v>
@@ -57266,7 +57266,7 @@
         <v>2086</v>
       </c>
       <c r="E1593">
-        <v>2086</v>
+        <v>1</v>
       </c>
       <c r="F1593" t="b">
         <v>0</v>
@@ -57682,7 +57682,7 @@
         <v>2101</v>
       </c>
       <c r="E1606">
-        <v>2101</v>
+        <v>1</v>
       </c>
       <c r="F1606" t="b">
         <v>0</v>
@@ -59042,7 +59042,7 @@
         <v>2090</v>
       </c>
       <c r="E1650">
-        <v>2090</v>
+        <v>1</v>
       </c>
       <c r="F1650" t="b">
         <v>0</v>
@@ -60646,7 +60646,7 @@
         <v>2107</v>
       </c>
       <c r="E1702">
-        <v>2107</v>
+        <v>1</v>
       </c>
       <c r="F1702" t="b">
         <v>0</v>
@@ -60806,7 +60806,7 @@
         <v>2092</v>
       </c>
       <c r="E1707">
-        <v>1</v>
+        <v>2092</v>
       </c>
       <c r="F1707" t="b">
         <v>0</v>
@@ -60838,7 +60838,7 @@
         <v>2100</v>
       </c>
       <c r="E1708">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F1708" t="b">
         <v>0</v>
@@ -61242,7 +61242,7 @@
         <v>2103</v>
       </c>
       <c r="E1724">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F1724" t="b">
         <v>0</v>
@@ -61538,7 +61538,7 @@
         <v>2104</v>
       </c>
       <c r="E1734">
-        <v>2104</v>
+        <v>1</v>
       </c>
       <c r="F1734" t="b">
         <v>0</v>
@@ -61666,7 +61666,7 @@
         <v>2105</v>
       </c>
       <c r="E1738">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F1738" t="b">
         <v>0</v>
@@ -62563,7 +62563,7 @@
         <v>2089</v>
       </c>
       <c r="E1768">
-        <v>1</v>
+        <v>2089</v>
       </c>
       <c r="F1768" t="b">
         <v>0</v>
@@ -62722,8 +62722,8 @@
       <c r="D1773">
         <v>2047</v>
       </c>
-      <c r="E1773" t="b">
-        <v>0</v>
+      <c r="E1773">
+        <v>2047</v>
       </c>
       <c r="F1773" t="b">
         <v>0</v>
@@ -62915,7 +62915,7 @@
         <v>2106</v>
       </c>
       <c r="E1779">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F1779" t="b">
         <v>0</v>
@@ -63559,7 +63559,7 @@
         <v>2079</v>
       </c>
       <c r="E1801">
-        <v>1</v>
+        <v>2079</v>
       </c>
       <c r="F1801" t="b">
         <v>0</v>
@@ -63655,7 +63655,7 @@
         <v>2044</v>
       </c>
       <c r="E1804">
-        <v>1</v>
+        <v>2044</v>
       </c>
       <c r="F1804" t="b">
         <v>0</v>
@@ -65099,7 +65099,7 @@
         <v>2094</v>
       </c>
       <c r="E1851">
-        <v>2094</v>
+        <v>1</v>
       </c>
       <c r="F1851" t="b">
         <v>0</v>
@@ -65575,7 +65575,7 @@
         <v>2108</v>
       </c>
       <c r="E1867">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F1867" t="b">
         <v>0</v>
@@ -66875,7 +66875,7 @@
         <v>2099</v>
       </c>
       <c r="E1908">
-        <v>1</v>
+        <v>2099</v>
       </c>
       <c r="F1908" t="b">
         <v>0</v>
@@ -67099,7 +67099,7 @@
         <v>2100</v>
       </c>
       <c r="E1915">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F1915" t="b">
         <v>0</v>
@@ -67631,7 +67631,7 @@
         <v>2053</v>
       </c>
       <c r="E1932">
-        <v>1</v>
+        <v>2053</v>
       </c>
       <c r="F1932" t="b">
         <v>0</v>
@@ -68844,7 +68844,7 @@
         <v>2069</v>
       </c>
       <c r="E1973">
-        <v>1</v>
+        <v>2069</v>
       </c>
       <c r="F1973" t="b">
         <v>0</v>
@@ -69612,7 +69612,7 @@
         <v>2103</v>
       </c>
       <c r="E1997">
-        <v>1</v>
+        <v>2103</v>
       </c>
       <c r="F1997" t="b">
         <v>0</v>
@@ -69804,7 +69804,7 @@
         <v>2105</v>
       </c>
       <c r="E2003">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F2003" t="b">
         <v>0</v>
@@ -69836,7 +69836,7 @@
         <v>2106</v>
       </c>
       <c r="E2004">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F2004" t="b">
         <v>0</v>
@@ -69996,7 +69996,7 @@
         <v>2107</v>
       </c>
       <c r="E2009">
-        <v>1</v>
+        <v>2107</v>
       </c>
       <c r="F2009" t="b">
         <v>0</v>
@@ -70124,7 +70124,7 @@
         <v>2108</v>
       </c>
       <c r="E2013">
-        <v>2108</v>
+        <v>1</v>
       </c>
       <c r="F2013" t="b">
         <v>0</v>
@@ -70316,7 +70316,7 @@
         <v>2109</v>
       </c>
       <c r="E2019">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F2019" t="b">
         <v>0</v>
@@ -70528,7 +70528,7 @@
         <v>2084</v>
       </c>
       <c r="E2026">
-        <v>1</v>
+        <v>2084</v>
       </c>
       <c r="F2026" t="b">
         <v>0</v>
@@ -70624,7 +70624,7 @@
         <v>2086</v>
       </c>
       <c r="E2029">
-        <v>2086</v>
+        <v>1</v>
       </c>
       <c r="F2029" t="b">
         <v>0</v>
@@ -70740,7 +70740,7 @@
         <v>2097</v>
       </c>
       <c r="E2033">
-        <v>2097</v>
+        <v>1</v>
       </c>
       <c r="F2033" t="b">
         <v>0</v>
@@ -70804,7 +70804,7 @@
         <v>2080</v>
       </c>
       <c r="E2035">
-        <v>2080</v>
+        <v>1</v>
       </c>
       <c r="F2035" t="b">
         <v>0</v>
@@ -70868,7 +70868,7 @@
         <v>2098</v>
       </c>
       <c r="E2037">
-        <v>2098</v>
+        <v>1</v>
       </c>
       <c r="F2037" t="b">
         <v>0</v>
@@ -71592,7 +71592,7 @@
         <v>2078</v>
       </c>
       <c r="E2060">
-        <v>2078</v>
+        <v>1</v>
       </c>
       <c r="F2060" t="b">
         <v>0</v>
@@ -72380,7 +72380,7 @@
         <v>2103</v>
       </c>
       <c r="E2085">
-        <v>2103</v>
+        <v>1</v>
       </c>
       <c r="F2085" t="b">
         <v>0</v>
@@ -72444,7 +72444,7 @@
         <v>2104</v>
       </c>
       <c r="E2087">
-        <v>1</v>
+        <v>2104</v>
       </c>
       <c r="F2087" t="b">
         <v>0</v>
@@ -72572,7 +72572,7 @@
         <v>2089</v>
       </c>
       <c r="E2091">
-        <v>1</v>
+        <v>2089</v>
       </c>
       <c r="F2091" t="b">
         <v>0</v>
@@ -72700,7 +72700,7 @@
         <v>2105</v>
       </c>
       <c r="E2095">
-        <v>2105</v>
+        <v>1</v>
       </c>
       <c r="F2095" t="b">
         <v>0</v>
@@ -72828,7 +72828,7 @@
         <v>2080</v>
       </c>
       <c r="E2099">
-        <v>1</v>
+        <v>2080</v>
       </c>
       <c r="F2099" t="b">
         <v>0</v>
@@ -73084,7 +73084,7 @@
         <v>2106</v>
       </c>
       <c r="E2107">
-        <v>1</v>
+        <v>2106</v>
       </c>
       <c r="F2107" t="b">
         <v>0</v>
@@ -73180,7 +73180,7 @@
         <v>2108</v>
       </c>
       <c r="E2110">
-        <v>1</v>
+        <v>2108</v>
       </c>
       <c r="F2110" t="b">
         <v>0</v>
@@ -73211,8 +73211,8 @@
       <c r="D2111">
         <v>2093</v>
       </c>
-      <c r="E2111">
-        <v>2093</v>
+      <c r="E2111" t="b">
+        <v>0</v>
       </c>
       <c r="F2111" t="b">
         <v>0</v>
@@ -73468,7 +73468,7 @@
         <v>2109</v>
       </c>
       <c r="E2119">
-        <v>2109</v>
+        <v>1</v>
       </c>
       <c r="F2119" t="b">
         <v>0</v>
@@ -73808,7 +73808,7 @@
         <v>2100</v>
       </c>
       <c r="E2130">
-        <v>2100</v>
+        <v>1</v>
       </c>
       <c r="F2130" t="b">
         <v>0</v>
@@ -74244,7 +74244,7 @@
         <v>2105</v>
       </c>
       <c r="E2144">
-        <v>1</v>
+        <v>2105</v>
       </c>
       <c r="F2144" t="b">
         <v>0</v>

</xml_diff>